<commit_message>
Converted tiles to billboards; added lighting on the maps; started on door logic
</commit_message>
<xml_diff>
--- a/Assets/Maps/TestMap.xlsx
+++ b/Assets/Maps/TestMap.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio\tfs\Spacialist\Assets\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Spacialist\Assets\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="6">
+  <si>
+    <t>1|L</t>
+  </si>
+  <si>
+    <t>1|LT</t>
+  </si>
+  <si>
+    <t>1|T</t>
+  </si>
+  <si>
+    <t>1||D4EFFF</t>
+  </si>
+  <si>
+    <t>1||FFFBC5</t>
+  </si>
+  <si>
+    <t>1|L|D4EFFF</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,14 +86,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -397,16 +413,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AF60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF21" sqref="AF21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="3.140625" style="1"/>
+    <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L2" s="1">
         <v>1</v>
       </c>
@@ -438,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L3" s="1">
         <v>1</v>
       </c>
@@ -470,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K4" s="1">
         <v>1</v>
       </c>
@@ -508,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K5" s="1">
         <v>1</v>
       </c>
@@ -546,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K6" s="1">
         <v>1</v>
       </c>
@@ -584,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J7" s="1">
         <v>1</v>
       </c>
@@ -628,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J8" s="1">
         <v>1</v>
       </c>
@@ -672,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J9" s="1">
         <v>1</v>
       </c>
@@ -716,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="1">
         <v>1</v>
       </c>
@@ -726,38 +742,38 @@
       <c r="K10" s="1">
         <v>1</v>
       </c>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1</v>
-      </c>
-      <c r="O10" s="1">
-        <v>1</v>
-      </c>
-      <c r="P10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1</v>
-      </c>
-      <c r="R10" s="1">
-        <v>1</v>
-      </c>
-      <c r="S10" s="1">
-        <v>1</v>
-      </c>
-      <c r="T10" s="1">
-        <v>1</v>
-      </c>
-      <c r="U10" s="1">
-        <v>1</v>
-      </c>
-      <c r="V10" s="1">
-        <v>1</v>
+      <c r="L10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W10" s="1">
         <v>1</v>
@@ -766,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
         <v>1</v>
       </c>
@@ -776,38 +792,38 @@
       <c r="K11" s="1">
         <v>1</v>
       </c>
-      <c r="L11" s="1">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1">
-        <v>1</v>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
       </c>
-      <c r="Q11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1">
-        <v>1</v>
+      <c r="Q11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S11" s="1">
         <v>1</v>
       </c>
-      <c r="T11" s="1">
-        <v>1</v>
+      <c r="T11" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U11" s="1">
         <v>1</v>
       </c>
-      <c r="V11" s="1">
-        <v>1</v>
+      <c r="V11" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W11" s="1">
         <v>1</v>
@@ -816,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="1">
         <v>1</v>
       </c>
@@ -826,8 +842,8 @@
       <c r="K12" s="1">
         <v>1</v>
       </c>
-      <c r="L12" s="1">
-        <v>1</v>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M12" s="1">
         <v>1</v>
@@ -841,8 +857,8 @@
       <c r="P12" s="1">
         <v>1</v>
       </c>
-      <c r="Q12" s="1">
-        <v>1</v>
+      <c r="Q12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R12" s="1">
         <v>1</v>
@@ -856,8 +872,8 @@
       <c r="U12" s="1">
         <v>1</v>
       </c>
-      <c r="V12" s="1">
-        <v>1</v>
+      <c r="V12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W12" s="1">
         <v>1</v>
@@ -866,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I13" s="1">
         <v>1</v>
       </c>
@@ -876,38 +892,38 @@
       <c r="K13" s="1">
         <v>1</v>
       </c>
-      <c r="L13" s="1">
-        <v>1</v>
+      <c r="L13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>1</v>
       </c>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1">
-        <v>1</v>
-      </c>
-      <c r="S13" s="1">
-        <v>1</v>
-      </c>
-      <c r="T13" s="1">
-        <v>1</v>
+      <c r="N13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U13" s="1">
         <v>1</v>
       </c>
-      <c r="V13" s="1">
-        <v>1</v>
+      <c r="V13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <v>1</v>
@@ -916,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="1">
         <v>1</v>
       </c>
@@ -926,38 +942,38 @@
       <c r="K14" s="1">
         <v>1</v>
       </c>
-      <c r="L14" s="1">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1</v>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P14" s="1">
         <v>1</v>
       </c>
-      <c r="Q14" s="1">
-        <v>1</v>
-      </c>
-      <c r="R14" s="1">
-        <v>1</v>
+      <c r="Q14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S14" s="1">
         <v>1</v>
       </c>
-      <c r="T14" s="1">
-        <v>1</v>
+      <c r="T14" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U14" s="1">
         <v>1</v>
       </c>
-      <c r="V14" s="1">
-        <v>1</v>
+      <c r="V14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W14" s="1">
         <v>1</v>
@@ -966,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="1">
         <v>1</v>
       </c>
@@ -976,8 +992,8 @@
       <c r="K15" s="1">
         <v>1</v>
       </c>
-      <c r="L15" s="1">
-        <v>1</v>
+      <c r="L15" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M15" s="1">
         <v>1</v>
@@ -991,8 +1007,8 @@
       <c r="P15" s="1">
         <v>1</v>
       </c>
-      <c r="Q15" s="1">
-        <v>1</v>
+      <c r="Q15" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R15" s="1">
         <v>1</v>
@@ -1006,8 +1022,8 @@
       <c r="U15" s="1">
         <v>1</v>
       </c>
-      <c r="V15" s="1">
-        <v>1</v>
+      <c r="V15" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W15" s="1">
         <v>1</v>
@@ -1016,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="1">
         <v>1</v>
       </c>
@@ -1026,38 +1042,38 @@
       <c r="K16" s="1">
         <v>1</v>
       </c>
-      <c r="L16" s="1">
-        <v>1</v>
+      <c r="L16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M16" s="1">
         <v>1</v>
       </c>
-      <c r="N16" s="1">
-        <v>1</v>
-      </c>
-      <c r="O16" s="1">
-        <v>1</v>
-      </c>
-      <c r="P16" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1</v>
-      </c>
-      <c r="S16" s="1">
-        <v>1</v>
-      </c>
-      <c r="T16" s="1">
-        <v>1</v>
+      <c r="N16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U16" s="1">
         <v>1</v>
       </c>
-      <c r="V16" s="1">
-        <v>1</v>
+      <c r="V16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W16" s="1">
         <v>1</v>
@@ -1066,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="1">
         <v>1</v>
       </c>
@@ -1076,38 +1092,38 @@
       <c r="K17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="1">
-        <v>1</v>
-      </c>
-      <c r="M17" s="1">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="O17" s="1">
-        <v>1</v>
+      <c r="L17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P17" s="1">
         <v>1</v>
       </c>
-      <c r="Q17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1">
-        <v>1</v>
+      <c r="Q17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S17" s="1">
         <v>1</v>
       </c>
-      <c r="T17" s="1">
-        <v>1</v>
+      <c r="T17" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U17" s="1">
         <v>1</v>
       </c>
-      <c r="V17" s="1">
-        <v>1</v>
+      <c r="V17" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W17" s="1">
         <v>1</v>
@@ -1116,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I18" s="1">
         <v>1</v>
       </c>
@@ -1126,8 +1142,8 @@
       <c r="K18" s="1">
         <v>1</v>
       </c>
-      <c r="L18" s="1">
-        <v>1</v>
+      <c r="L18" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M18" s="1">
         <v>1</v>
@@ -1141,8 +1157,8 @@
       <c r="P18" s="1">
         <v>1</v>
       </c>
-      <c r="Q18" s="1">
-        <v>1</v>
+      <c r="Q18" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R18" s="1">
         <v>1</v>
@@ -1156,8 +1172,8 @@
       <c r="U18" s="1">
         <v>1</v>
       </c>
-      <c r="V18" s="1">
-        <v>1</v>
+      <c r="V18" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W18" s="1">
         <v>1</v>
@@ -1166,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I19" s="1">
         <v>1</v>
       </c>
@@ -1176,38 +1192,38 @@
       <c r="K19" s="1">
         <v>1</v>
       </c>
-      <c r="L19" s="1">
-        <v>1</v>
+      <c r="L19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M19" s="1">
         <v>1</v>
       </c>
-      <c r="N19" s="1">
-        <v>1</v>
-      </c>
-      <c r="O19" s="1">
-        <v>1</v>
-      </c>
-      <c r="P19" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>1</v>
-      </c>
-      <c r="R19" s="1">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1">
-        <v>1</v>
-      </c>
-      <c r="T19" s="1">
-        <v>1</v>
+      <c r="N19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U19" s="1">
         <v>1</v>
       </c>
-      <c r="V19" s="1">
-        <v>1</v>
+      <c r="V19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W19" s="1">
         <v>1</v>
@@ -1216,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I20" s="1">
         <v>1</v>
       </c>
@@ -1226,38 +1242,38 @@
       <c r="K20" s="1">
         <v>1</v>
       </c>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
-      <c r="M20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1">
-        <v>1</v>
-      </c>
-      <c r="O20" s="1">
-        <v>1</v>
+      <c r="L20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P20" s="1">
         <v>1</v>
       </c>
-      <c r="Q20" s="1">
-        <v>1</v>
-      </c>
-      <c r="R20" s="1">
-        <v>1</v>
+      <c r="Q20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S20" s="1">
         <v>1</v>
       </c>
-      <c r="T20" s="1">
-        <v>1</v>
+      <c r="T20" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U20" s="1">
         <v>1</v>
       </c>
-      <c r="V20" s="1">
-        <v>1</v>
+      <c r="V20" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W20" s="1">
         <v>1</v>
@@ -1266,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="1">
         <v>1</v>
       </c>
@@ -1276,8 +1292,8 @@
       <c r="K21" s="1">
         <v>1</v>
       </c>
-      <c r="L21" s="1">
-        <v>1</v>
+      <c r="L21" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M21" s="1">
         <v>1</v>
@@ -1291,8 +1307,8 @@
       <c r="P21" s="1">
         <v>1</v>
       </c>
-      <c r="Q21" s="1">
-        <v>1</v>
+      <c r="Q21" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R21" s="1">
         <v>1</v>
@@ -1306,8 +1322,8 @@
       <c r="U21" s="1">
         <v>1</v>
       </c>
-      <c r="V21" s="1">
-        <v>1</v>
+      <c r="V21" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W21" s="1">
         <v>1</v>
@@ -1316,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="1">
         <v>1</v>
       </c>
@@ -1326,38 +1342,38 @@
       <c r="K22" s="1">
         <v>1</v>
       </c>
-      <c r="L22" s="1">
-        <v>1</v>
+      <c r="L22" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M22" s="1">
         <v>1</v>
       </c>
-      <c r="N22" s="1">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1</v>
-      </c>
-      <c r="P22" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>1</v>
-      </c>
-      <c r="R22" s="1">
-        <v>1</v>
-      </c>
-      <c r="S22" s="1">
-        <v>1</v>
-      </c>
-      <c r="T22" s="1">
-        <v>1</v>
+      <c r="N22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U22" s="1">
         <v>1</v>
       </c>
-      <c r="V22" s="1">
-        <v>1</v>
+      <c r="V22" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W22" s="1">
         <v>1</v>
@@ -1366,7 +1382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="1">
         <v>1</v>
       </c>
@@ -1376,38 +1392,38 @@
       <c r="K23" s="1">
         <v>1</v>
       </c>
-      <c r="L23" s="1">
-        <v>1</v>
-      </c>
-      <c r="M23" s="1">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1">
-        <v>1</v>
+      <c r="L23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P23" s="1">
         <v>1</v>
       </c>
-      <c r="Q23" s="1">
-        <v>1</v>
-      </c>
-      <c r="R23" s="1">
-        <v>1</v>
+      <c r="Q23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S23" s="1">
         <v>1</v>
       </c>
-      <c r="T23" s="1">
-        <v>1</v>
+      <c r="T23" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U23" s="1">
         <v>1</v>
       </c>
-      <c r="V23" s="1">
-        <v>1</v>
+      <c r="V23" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W23" s="1">
         <v>1</v>
@@ -1416,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="1">
         <v>1</v>
       </c>
@@ -1426,8 +1442,8 @@
       <c r="K24" s="1">
         <v>1</v>
       </c>
-      <c r="L24" s="1">
-        <v>1</v>
+      <c r="L24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M24" s="1">
         <v>1</v>
@@ -1441,8 +1457,8 @@
       <c r="P24" s="1">
         <v>1</v>
       </c>
-      <c r="Q24" s="1">
-        <v>1</v>
+      <c r="Q24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>1</v>
@@ -1456,8 +1472,8 @@
       <c r="U24" s="1">
         <v>1</v>
       </c>
-      <c r="V24" s="1">
-        <v>1</v>
+      <c r="V24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W24" s="1">
         <v>1</v>
@@ -1466,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="1">
         <v>1</v>
       </c>
@@ -1476,38 +1492,38 @@
       <c r="K25" s="1">
         <v>1</v>
       </c>
-      <c r="L25" s="1">
-        <v>1</v>
+      <c r="L25" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M25" s="1">
         <v>1</v>
       </c>
-      <c r="N25" s="1">
-        <v>1</v>
-      </c>
-      <c r="O25" s="1">
-        <v>1</v>
-      </c>
-      <c r="P25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1">
-        <v>1</v>
-      </c>
-      <c r="S25" s="1">
-        <v>1</v>
-      </c>
-      <c r="T25" s="1">
-        <v>1</v>
+      <c r="N25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U25" s="1">
         <v>1</v>
       </c>
-      <c r="V25" s="1">
-        <v>1</v>
+      <c r="V25" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W25" s="1">
         <v>1</v>
@@ -1516,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="1">
         <v>1</v>
       </c>
@@ -1526,38 +1542,38 @@
       <c r="K26" s="1">
         <v>1</v>
       </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1">
-        <v>1</v>
-      </c>
-      <c r="O26" s="1">
-        <v>1</v>
+      <c r="L26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P26" s="1">
         <v>1</v>
       </c>
-      <c r="Q26" s="1">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1">
-        <v>1</v>
+      <c r="Q26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S26" s="1">
         <v>1</v>
       </c>
-      <c r="T26" s="1">
-        <v>1</v>
+      <c r="T26" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U26" s="1">
         <v>1</v>
       </c>
-      <c r="V26" s="1">
-        <v>1</v>
+      <c r="V26" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W26" s="1">
         <v>1</v>
@@ -1566,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="1">
         <v>1</v>
       </c>
@@ -1576,8 +1592,8 @@
       <c r="K27" s="1">
         <v>1</v>
       </c>
-      <c r="L27" s="1">
-        <v>1</v>
+      <c r="L27" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M27" s="1">
         <v>1</v>
@@ -1591,8 +1607,8 @@
       <c r="P27" s="1">
         <v>1</v>
       </c>
-      <c r="Q27" s="1">
-        <v>1</v>
+      <c r="Q27" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R27" s="1">
         <v>1</v>
@@ -1606,8 +1622,8 @@
       <c r="U27" s="1">
         <v>1</v>
       </c>
-      <c r="V27" s="1">
-        <v>1</v>
+      <c r="V27" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W27" s="1">
         <v>1</v>
@@ -1616,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="1">
         <v>1</v>
       </c>
@@ -1626,38 +1642,38 @@
       <c r="K28" s="1">
         <v>1</v>
       </c>
-      <c r="L28" s="1">
-        <v>1</v>
+      <c r="L28" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M28" s="1">
         <v>1</v>
       </c>
-      <c r="N28" s="1">
-        <v>1</v>
-      </c>
-      <c r="O28" s="1">
-        <v>1</v>
-      </c>
-      <c r="P28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>1</v>
-      </c>
-      <c r="R28" s="1">
-        <v>1</v>
-      </c>
-      <c r="S28" s="1">
-        <v>1</v>
-      </c>
-      <c r="T28" s="1">
-        <v>1</v>
+      <c r="N28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U28" s="1">
         <v>1</v>
       </c>
-      <c r="V28" s="1">
-        <v>1</v>
+      <c r="V28" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W28" s="1">
         <v>1</v>
@@ -1666,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="1">
         <v>1</v>
       </c>
@@ -1676,38 +1692,38 @@
       <c r="K29" s="1">
         <v>1</v>
       </c>
-      <c r="L29" s="1">
-        <v>1</v>
-      </c>
-      <c r="M29" s="1">
-        <v>1</v>
-      </c>
-      <c r="N29" s="1">
-        <v>1</v>
-      </c>
-      <c r="O29" s="1">
-        <v>1</v>
+      <c r="L29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P29" s="1">
         <v>1</v>
       </c>
-      <c r="Q29" s="1">
-        <v>1</v>
-      </c>
-      <c r="R29" s="1">
-        <v>1</v>
+      <c r="Q29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S29" s="1">
         <v>1</v>
       </c>
-      <c r="T29" s="1">
-        <v>1</v>
+      <c r="T29" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="U29" s="1">
         <v>1</v>
       </c>
-      <c r="V29" s="1">
-        <v>1</v>
+      <c r="V29" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W29" s="1">
         <v>1</v>
@@ -1716,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I30" s="1">
         <v>1</v>
       </c>
@@ -1726,8 +1742,8 @@
       <c r="K30" s="1">
         <v>1</v>
       </c>
-      <c r="L30" s="1">
-        <v>1</v>
+      <c r="L30" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M30" s="1">
         <v>1</v>
@@ -1741,8 +1757,8 @@
       <c r="P30" s="1">
         <v>1</v>
       </c>
-      <c r="Q30" s="1">
-        <v>1</v>
+      <c r="Q30" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R30" s="1">
         <v>1</v>
@@ -1756,8 +1772,8 @@
       <c r="U30" s="1">
         <v>1</v>
       </c>
-      <c r="V30" s="1">
-        <v>1</v>
+      <c r="V30" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W30" s="1">
         <v>1</v>
@@ -1766,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="1">
         <v>1</v>
       </c>
@@ -1776,38 +1792,38 @@
       <c r="K31" s="1">
         <v>1</v>
       </c>
-      <c r="L31" s="1">
-        <v>1</v>
+      <c r="L31" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M31" s="1">
         <v>1</v>
       </c>
-      <c r="N31" s="1">
-        <v>1</v>
-      </c>
-      <c r="O31" s="1">
-        <v>1</v>
-      </c>
-      <c r="P31" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>1</v>
-      </c>
-      <c r="R31" s="1">
-        <v>1</v>
-      </c>
-      <c r="S31" s="1">
-        <v>1</v>
-      </c>
-      <c r="T31" s="1">
-        <v>1</v>
+      <c r="N31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U31" s="1">
         <v>1</v>
       </c>
-      <c r="V31" s="1">
-        <v>1</v>
+      <c r="V31" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W31" s="1">
         <v>1</v>
@@ -1816,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="9:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="1">
         <v>1</v>
       </c>
@@ -1826,14 +1842,14 @@
       <c r="K32" s="1">
         <v>1</v>
       </c>
-      <c r="L32" s="1">
-        <v>1</v>
+      <c r="L32" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M32" s="1">
         <v>1</v>
       </c>
-      <c r="N32" s="1">
-        <v>1</v>
+      <c r="N32" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O32" s="1">
         <v>1</v>
@@ -1841,8 +1857,8 @@
       <c r="P32" s="1">
         <v>1</v>
       </c>
-      <c r="Q32" s="1">
-        <v>1</v>
+      <c r="Q32" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R32" s="1">
         <v>1</v>
@@ -1850,14 +1866,14 @@
       <c r="S32" s="1">
         <v>1</v>
       </c>
-      <c r="T32" s="1">
-        <v>1</v>
+      <c r="T32" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U32" s="1">
         <v>1</v>
       </c>
-      <c r="V32" s="1">
-        <v>1</v>
+      <c r="V32" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="W32" s="1">
         <v>1</v>
@@ -1866,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H33" s="1">
         <v>1</v>
       </c>
@@ -1922,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G34" s="1">
         <v>1</v>
       </c>
@@ -1984,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F35" s="1">
         <v>1</v>
       </c>
@@ -2052,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="1">
         <v>1</v>
       </c>
@@ -2126,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>1</v>
       </c>
@@ -2206,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>1</v>
       </c>
@@ -2292,7 +2308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>1</v>
       </c>
@@ -2384,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -2482,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -2580,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2678,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -2776,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -2874,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -2972,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -3070,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -3168,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -3266,7 +3282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -3364,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -3462,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1</v>
       </c>
@@ -3560,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>1</v>
       </c>
@@ -3658,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -3756,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>1</v>
       </c>
@@ -3854,7 +3870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1</v>
       </c>
@@ -3952,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>1</v>
       </c>
@@ -4038,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E57" s="1">
         <v>1</v>
       </c>
@@ -4112,7 +4128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G58" s="1">
         <v>1</v>
       </c>
@@ -4174,7 +4190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I59" s="1">
         <v>1</v>
       </c>
@@ -4224,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I60" s="1">
         <v>2</v>
       </c>
@@ -4252,10 +4268,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>